<commit_message>
Code compiled, results available
</commit_message>
<xml_diff>
--- a/1. ARIMAX/ARIMAX_results_pre.xlsx
+++ b/1. ARIMAX/ARIMAX_results_pre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1128,6 +1128,582 @@
         <v>62.93436293436293</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.262249820071284</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3.333893823378794</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.00974046742299407</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.624031007751938</v>
+      </c>
+      <c r="J20" t="n">
+        <v>57.14285714285714</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>PEP</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.2695588772136407</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.2035406185491022</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.009050882111654309</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.5465116279069767</v>
+      </c>
+      <c r="J21" t="n">
+        <v>66.40926640926641</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>KRU</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2.618842383902459</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2.001682927551309</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.01239655736930432</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.6162790697674418</v>
+      </c>
+      <c r="J22" t="n">
+        <v>50.57915057915058</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NEU</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3.581292169103917</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.662951816310947</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.008951901977750894</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.5542635658914729</v>
+      </c>
+      <c r="J23" t="n">
+        <v>64.09266409266409</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ERB</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2852847340679718</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2023870455546976</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.01512462150663506</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.5155038759689923</v>
+      </c>
+      <c r="J24" t="n">
+        <v>44.01544401544402</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ATD</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0483899941386483</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.03401734566914823</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.009197572952402472</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.3798449612403101</v>
+      </c>
+      <c r="J25" t="n">
+        <v>66.02316602316603</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>DAT</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1.522083412802567</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.021068681763854</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.02907598781905718</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.3488372093023256</v>
+      </c>
+      <c r="J26" t="n">
+        <v>25.86872586872587</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ZMT</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.02576193131210118</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.0147605819817843</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.01730472196972008</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.1937984496124031</v>
+      </c>
+      <c r="J27" t="n">
+        <v>60.61776061776062</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>KTY</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4.980710419265365</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3.693641805455617</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.01117038338088966</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.4651162790697674</v>
+      </c>
+      <c r="J28" t="n">
+        <v>57.14285714285714</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ABE</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>10</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.3728079688391112</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.2667566143420379</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.0136428731980587</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.4224806201550387</v>
+      </c>
+      <c r="J29" t="n">
+        <v>49.03474903474903</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>MRB</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>8</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.01841025824737029</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.01405469968690697</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.013908950877897</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.4573643410852713</v>
+      </c>
+      <c r="J30" t="n">
+        <v>46.71814671814672</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>10</v>
+      </c>
+      <c r="E31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.0693466576127281</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.05262296550380359</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.008515165414469669</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.5503875968992248</v>
+      </c>
+      <c r="J31" t="n">
+        <v>66.40926640926641</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>WIG</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" t="n">
+        <v>548.6331449524837</v>
+      </c>
+      <c r="G32" t="n">
+        <v>439.626471200701</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.007561880183372149</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.7015503875968992</v>
+      </c>
+      <c r="J32" t="n">
+        <v>73.35907335907336</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>WIG20</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>15.96880173581907</v>
+      </c>
+      <c r="G33" t="n">
+        <v>12.38793411847845</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.005499783806024364</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.6511627906976745</v>
+      </c>
+      <c r="J33" t="n">
+        <v>85.71428571428571</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>mWIG40</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>3</v>
+      </c>
+      <c r="E34" t="n">
+        <v>4</v>
+      </c>
+      <c r="F34" t="n">
+        <v>21.18662715589623</v>
+      </c>
+      <c r="G34" t="n">
+        <v>16.47272245773662</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.004148136970349986</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.6744186046511628</v>
+      </c>
+      <c r="J34" t="n">
+        <v>93.43629343629344</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ARIMAX</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>sWIG80</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>7</v>
+      </c>
+      <c r="E35" t="n">
+        <v>9</v>
+      </c>
+      <c r="F35" t="n">
+        <v>221.5425959676884</v>
+      </c>
+      <c r="G35" t="n">
+        <v>187.5055945082987</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.01599344015247646</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.7209302325581395</v>
+      </c>
+      <c r="J35" t="n">
+        <v>32.81853281853282</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>